<commit_message>
update for current gameweek
</commit_message>
<xml_diff>
--- a/current_gw_fixtures.xlsx
+++ b/current_gw_fixtures.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,103 +463,103 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Leicester City - West Ham United</t>
+          <t>VfL Bochum 1848 - SV Werder Bremen</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.67</t>
+          <t>1.42</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3.17</t>
+          <t>4.25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.42</t>
+          <t>9.75</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Bundesliga</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Newcastle United - Liverpool</t>
+          <t>Borussia Monchengladbach - Borussia Dortmund</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.35</t>
+          <t>2.18</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.08</t>
+          <t>3.08</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12.42</t>
+          <t>9.08</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Bundesliga</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Southampton - Chelsea</t>
+          <t>VfL Wolfsburg - 1. FSV Mainz 05</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.48</t>
+          <t>1.44</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5.50</t>
+          <t>3.92</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9.58</t>
+          <t>9.67</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Bundesliga</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VfB Stuttgart - 1. FC Union Berlin</t>
+          <t>TSG Hoffenheim - SC Freiburg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2.88</t>
+          <t>1.58</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3.58</t>
+          <t>2.83</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9.00</t>
+          <t>8.25</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -571,184 +571,184 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>VfL Bochum 1848 - SV Werder Bremen</t>
+          <t>Crystal Palace - Manchester City</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.42</t>
+          <t>1.60</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.25</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>9.75</t>
+          <t>9.83</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Premier League</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Borussia Monchengladbach - Borussia Dortmund</t>
+          <t>Aston Villa - Southampton</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2.18</t>
+          <t>0.93</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3.08</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>9.08</t>
+          <t>11.17</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Premier League</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VfL Wolfsburg - 1. FSV Mainz 05</t>
+          <t>Leicester City - Brighton Hove Albion</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.44</t>
+          <t>1.63</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3.92</t>
+          <t>3.42</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>9.67</t>
+          <t>9.75</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Premier League</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TSG Hoffenheim - SC Freiburg</t>
+          <t>Fulham - Arsenal</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.58</t>
+          <t>1.39</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2.83</t>
+          <t>3.75</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>8.25</t>
+          <t>10.92</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Premier League</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sheffield Wednesday - Preston North End</t>
+          <t>Tottenham Hotspur - Chelsea</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.15</t>
+          <t>1.36</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.08</t>
+          <t>4.17</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10.33</t>
+          <t>11.33</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>EFL Championship</t>
+          <t>Premier League</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Leeds United - Derby County</t>
+          <t>West Ham United - Wolverhampton Wanderers</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1.71</t>
+          <t>1.35</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4.25</t>
+          <t>3.83</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>9.08</t>
+          <t>9.58</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>EFL Championship</t>
+          <t>Premier League</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Luton Town - Swansea City</t>
+          <t>Sheffield Wednesday - Preston North End</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1.46</t>
+          <t>1.15</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.67</t>
+          <t>3.08</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>8.83</t>
+          <t>10.33</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -760,22 +760,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cardiff City - Watford</t>
+          <t>Leeds United - Derby County</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.28</t>
+          <t>1.71</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.17</t>
+          <t>4.25</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11.33</t>
+          <t>9.08</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -787,22 +787,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Millwall - Coventry City</t>
+          <t>Luton Town - Swansea City</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.30</t>
+          <t>1.46</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4.33</t>
+          <t>3.67</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.25</t>
+          <t>8.83</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -814,22 +814,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hull City - Blackburn Rovers</t>
+          <t>Cardiff City - Watford</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1.88</t>
+          <t>1.28</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3.42</t>
+          <t>4.17</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>10.83</t>
+          <t>11.33</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -841,341 +841,341 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Inter Milan - Parma</t>
+          <t>Queens Park Rangers - Norwich City</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1.54</t>
+          <t>1.92</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3.58</t>
+          <t>4.08</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>9.75</t>
+          <t>12.25</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Serie A</t>
+          <t>EFL Championship</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Genoa - Torino</t>
+          <t>Millwall - Coventry City</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2.38</t>
+          <t>1.30</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4.92</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>9.17</t>
+          <t>10.25</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Serie A</t>
+          <t>EFL Championship</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Juventus - Bologna</t>
+          <t>Hull City - Blackburn Rovers</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1.48</t>
+          <t>1.88</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3.92</t>
+          <t>3.42</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>7.25</t>
+          <t>10.83</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Serie A</t>
+          <t>EFL Championship</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Moreirense - Sporting CP</t>
+          <t>Inter Milan - Parma</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.98</t>
+          <t>1.54</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5.17</t>
+          <t>3.58</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>9.25</t>
+          <t>9.75</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Primera Division</t>
+          <t>Serie A</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sporting Braga - Estoril</t>
+          <t>Atalanta - AC Milan</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1.19</t>
+          <t>1.56</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4.25</t>
+          <t>3.92</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11.58</t>
+          <t>8.08</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Primera Division</t>
+          <t>Serie A</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LOSC Lille - Stade Brestois 29</t>
+          <t>Genoa - Torino</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0.98</t>
+          <t>2.38</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4.33</t>
+          <t>4.92</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8.83</t>
+          <t>9.17</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Ligue 1</t>
+          <t>Serie A</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RC Lens - Montpellier Hérault SC</t>
+          <t>Juventus - Bologna</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1.02</t>
+          <t>1.48</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4.75</t>
+          <t>3.92</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>8.50</t>
+          <t>7.25</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ligue 1</t>
+          <t>Serie A</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RC Strasbourg Alsace - Stade DE Reims</t>
+          <t>AS Roma - Lecce</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1.35</t>
+          <t>1.17</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>3.50</t>
+          <t>4.67</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>8.42</t>
+          <t>8.92</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Ligue 1</t>
+          <t>Serie A</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AS Saint-Étienne - Marseille</t>
+          <t>RC Celta - RCD Mallorca</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1.79</t>
+          <t>1.22</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>9.75</t>
+          <t>7.75</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Ligue 1</t>
+          <t>La Liga</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PSV Eindhoven - NEC Nijmegen</t>
+          <t>Valencia CF - Rayo Vallecano</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2.50</t>
+          <t>1.38</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.92</t>
+          <t>5.92</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>10.08</t>
+          <t>10.75</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Eredivisie</t>
+          <t>La Liga</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AZ Alkmaar - SC Heerenveen</t>
+          <t>Girona FC - Real Madrid</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.61</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>4.42</t>
+          <t>4.67</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10.42</t>
+          <t>7.50</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Eredivisie</t>
+          <t>La Liga</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Willem II - RKC Waalwijk</t>
+          <t>Athletic Club - Villarreal CF</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1.46</t>
+          <t>1.56</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3.50</t>
+          <t>6.17</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>9.83</t>
+          <t>8.50</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Eredivisie</t>
+          <t>La Liga</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AFC Ajax - FC Utrecht</t>
+          <t>LOSC Lille - Stade Brestois 29</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1.60</t>
+          <t>0.98</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>3.25</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1185,7 +1185,223 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Eredivisie</t>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>RC Strasbourg Alsace - Stade DE Reims</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>8.42</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>AS Saint-Étienne - Marseille</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>9.75</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Moreirense - Sporting CP</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0.98</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>5.17</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Primera Division</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Sporting Braga - Estoril</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>4.25</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>11.58</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Primera Division</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Benfica - Vitoria Guimaraes</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>4.75</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>10.92</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Primera Division</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Santa Clara - Rio Ave</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>1.31</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>7.08</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>9.25</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Primera Division</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>FC Famalicao - FC Porto</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2.08</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>5.25</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>9.00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Primera Division</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Boavista FC - SC Farense</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>10.75</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Primera Division</t>
         </is>
       </c>
     </row>

</xml_diff>